<commit_message>
Fixed the hit box not activating issue, changed charge states from bools to an enum
the excel has been updated to match.
</commit_message>
<xml_diff>
--- a/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
+++ b/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\musicGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\superMusicGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Boss</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Haydon ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           </t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>complete, the hitboxes are probably too big now that they actually work but that can be changed easily</t>
+  </si>
+  <si>
+    <t>these work now I think, just need to get good feel</t>
   </si>
 </sst>
 </file>
@@ -447,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,10 +473,10 @@
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -471,8 +486,11 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -482,8 +500,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -494,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -505,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -515,8 +536,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -527,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -537,8 +561,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -546,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -554,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -565,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -573,15 +600,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
       <c r="C12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -592,15 +622,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
       <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -608,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add Controller Spells and Health bar
</commit_message>
<xml_diff>
--- a/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
+++ b/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\superMusicGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\superMusicGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Boss</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>these work now I think, just need to get good feel</t>
+  </si>
+  <si>
+    <t>complete spells now work with the face buttons and you can attack with the left bumper or trigger</t>
+  </si>
+  <si>
+    <t>complete theres now a pretty basic health bar</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +531,9 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -549,6 +558,9 @@
       </c>
       <c r="C6">
         <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started 2p and started boss
boss is half broken - see excel
2p needs testing with second controller, honestly not sure if it works
or not
</commit_message>
<xml_diff>
--- a/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
+++ b/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\superMusicGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\superMusicGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Boss</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Haydon ?</t>
   </si>
   <si>
-    <t xml:space="preserve">           </t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -117,6 +114,15 @@
   </si>
   <si>
     <t>complete theres now a pretty basic health bar</t>
+  </si>
+  <si>
+    <t>think this is complete now, need to actually test with another controller though</t>
+  </si>
+  <si>
+    <t>tom</t>
+  </si>
+  <si>
+    <t>created class for boss, has health that player can decrease with sword swing, needs delay, is currently broken from players end, calls the lose hp for every frame of swing</t>
   </si>
 </sst>
 </file>
@@ -132,12 +138,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,8 +170,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +491,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,21 +513,21 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,75 +542,87 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,11 +648,11 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
       <c r="C12">
         <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
build wood wall blueprint (start), made option for turret to be random or fixed
</commit_message>
<xml_diff>
--- a/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
+++ b/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Boss</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>add decoration sprites</t>
+  </si>
+  <si>
+    <t>this is pretty much done, just want it to have a burning flipbook that plays before it gets destroyed</t>
   </si>
 </sst>
 </file>
@@ -521,13 +524,13 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -552,6 +555,9 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
endless spawners, trigger problem fixed, boss room trigger added, made changed to fireballs destroying things
made it so fireball will be destroyed but not kill the bats if they
aren't tired, so you cant just spam them ad eventually kill something,
also zombies don't destroy them anymore so they can get destroyed
</commit_message>
<xml_diff>
--- a/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
+++ b/TODOLISTPLEASEREADANDUPDSTELOTSXOXOX.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simhy007/Downloads/superMusicGame-master 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\superMusicGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Fix player swing hitboxes</t>
   </si>
@@ -195,12 +195,18 @@
   </si>
   <si>
     <t>FRIEND FIGHT</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">works now, is in player lose hp </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,19 +577,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="94.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -597,7 +603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -605,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -614,7 +620,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -625,7 +631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -633,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -644,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -655,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -666,16 +672,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -686,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -695,7 +706,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -703,15 +714,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -722,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -733,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -743,7 +760,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -754,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -765,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -773,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -784,7 +801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -794,7 +811,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -805,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -813,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -821,7 +838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -830,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -840,7 +857,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
@@ -850,7 +867,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -862,7 +879,7 @@
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -890,7 +907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -904,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -918,7 +935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -932,7 +949,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -946,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -960,7 +977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
@@ -974,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>

</xml_diff>